<commit_message>
Add codes for replication
</commit_message>
<xml_diff>
--- a/Data/Response_Rates_Data.xlsx
+++ b/Data/Response_Rates_Data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewcforrester/projects/JSM-2024-Analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0B1E96-F99F-114A-B79B-84691688B100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F76223-9D71-3F4B-AA19-3ED8E3488C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="780" windowWidth="30240" windowHeight="17980" xr2:uid="{AAC91AC4-385C-0D48-BC01-5D98CD21A098}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="17980" activeTab="4" xr2:uid="{AAC91AC4-385C-0D48-BC01-5D98CD21A098}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="SIPP" sheetId="4" r:id="rId2"/>
     <sheet name="DataNotes" sheetId="2" r:id="rId3"/>
     <sheet name="SSM" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="241">
   <si>
     <t>DataYear</t>
   </si>
@@ -426,6 +427,342 @@
   </si>
   <si>
     <t>FTF/CAPI</t>
+  </si>
+  <si>
+    <t>common_intercept</t>
+  </si>
+  <si>
+    <t>1.961***</t>
+  </si>
+  <si>
+    <t>1.391***</t>
+  </si>
+  <si>
+    <t>0.934***</t>
+  </si>
+  <si>
+    <t>1.282***</t>
+  </si>
+  <si>
+    <t>-0.591*</t>
+  </si>
+  <si>
+    <t>1.745*</t>
+  </si>
+  <si>
+    <t>2.268***</t>
+  </si>
+  <si>
+    <t>2.642***</t>
+  </si>
+  <si>
+    <t>1.956***</t>
+  </si>
+  <si>
+    <t>2.483***</t>
+  </si>
+  <si>
+    <t>1.841*</t>
+  </si>
+  <si>
+    <t>2.393***</t>
+  </si>
+  <si>
+    <t>3.427***</t>
+  </si>
+  <si>
+    <t>2.618***</t>
+  </si>
+  <si>
+    <t>3.236***</t>
+  </si>
+  <si>
+    <t>0.843*</t>
+  </si>
+  <si>
+    <t>0.818*</t>
+  </si>
+  <si>
+    <t>2.421***</t>
+  </si>
+  <si>
+    <t>3.265***</t>
+  </si>
+  <si>
+    <t>2.482***</t>
+  </si>
+  <si>
+    <t>3.078***</t>
+  </si>
+  <si>
+    <t>0.761*</t>
+  </si>
+  <si>
+    <t>0.744*</t>
+  </si>
+  <si>
+    <t>2.509***</t>
+  </si>
+  <si>
+    <t>2.103***</t>
+  </si>
+  <si>
+    <t>1.474***</t>
+  </si>
+  <si>
+    <t>1.953***</t>
+  </si>
+  <si>
+    <t>4.759***</t>
+  </si>
+  <si>
+    <t>4.352***</t>
+  </si>
+  <si>
+    <t>3.122***</t>
+  </si>
+  <si>
+    <t>-1.41**</t>
+  </si>
+  <si>
+    <t>2.042***</t>
+  </si>
+  <si>
+    <t>-3.041*</t>
+  </si>
+  <si>
+    <t>2.87***</t>
+  </si>
+  <si>
+    <t>-1.588***</t>
+  </si>
+  <si>
+    <t>4.779***</t>
+  </si>
+  <si>
+    <t>1.29***</t>
+  </si>
+  <si>
+    <t>-2.232***</t>
+  </si>
+  <si>
+    <t>-1.556***</t>
+  </si>
+  <si>
+    <t>-2.901*</t>
+  </si>
+  <si>
+    <t>1.093**</t>
+  </si>
+  <si>
+    <t>-2.325***</t>
+  </si>
+  <si>
+    <t>-1.373***</t>
+  </si>
+  <si>
+    <t>-1.383***</t>
+  </si>
+  <si>
+    <t>-1.44***</t>
+  </si>
+  <si>
+    <t>2.339**</t>
+  </si>
+  <si>
+    <t>6.545***</t>
+  </si>
+  <si>
+    <t>2.585***</t>
+  </si>
+  <si>
+    <t>-2.784***</t>
+  </si>
+  <si>
+    <t>-1.741***</t>
+  </si>
+  <si>
+    <t>1.314**</t>
+  </si>
+  <si>
+    <t>-4.894***</t>
+  </si>
+  <si>
+    <t>2.295***</t>
+  </si>
+  <si>
+    <t>-2.989***</t>
+  </si>
+  <si>
+    <t>-1.458**</t>
+  </si>
+  <si>
+    <t>-1.534**</t>
+  </si>
+  <si>
+    <t>-1.606**</t>
+  </si>
+  <si>
+    <t>1.549***</t>
+  </si>
+  <si>
+    <t>0.975***</t>
+  </si>
+  <si>
+    <t>0.631**</t>
+  </si>
+  <si>
+    <t>0.893***</t>
+  </si>
+  <si>
+    <t>6.5***</t>
+  </si>
+  <si>
+    <t>3.733***</t>
+  </si>
+  <si>
+    <t>-2.213***</t>
+  </si>
+  <si>
+    <t>2.326***</t>
+  </si>
+  <si>
+    <t>-3.868**</t>
+  </si>
+  <si>
+    <t>3.405***</t>
+  </si>
+  <si>
+    <t>-2.378***</t>
+  </si>
+  <si>
+    <t>1.995***</t>
+  </si>
+  <si>
+    <t>3.206***</t>
+  </si>
+  <si>
+    <t>0.778*</t>
+  </si>
+  <si>
+    <t>2.498***</t>
+  </si>
+  <si>
+    <t>3.036***</t>
+  </si>
+  <si>
+    <t>0.941**</t>
+  </si>
+  <si>
+    <t>0.922**</t>
+  </si>
+  <si>
+    <t>0.86**</t>
+  </si>
+  <si>
+    <t>1.55***</t>
+  </si>
+  <si>
+    <t>0.547*</t>
+  </si>
+  <si>
+    <t>-0.661**</t>
+  </si>
+  <si>
+    <t>-0.694**</t>
+  </si>
+  <si>
+    <t>1.797*</t>
+  </si>
+  <si>
+    <t>5.026***</t>
+  </si>
+  <si>
+    <t>11.514***</t>
+  </si>
+  <si>
+    <t>1.878*</t>
+  </si>
+  <si>
+    <t>3.704***</t>
+  </si>
+  <si>
+    <t>9.27***</t>
+  </si>
+  <si>
+    <t>10.941***</t>
+  </si>
+  <si>
+    <t>4.235***</t>
+  </si>
+  <si>
+    <t>7.113**</t>
+  </si>
+  <si>
+    <t>4.185***</t>
+  </si>
+  <si>
+    <t>3.958***</t>
+  </si>
+  <si>
+    <t>1.637***</t>
+  </si>
+  <si>
+    <t>-0.832***</t>
+  </si>
+  <si>
+    <t>-0.621**</t>
+  </si>
+  <si>
+    <t>-0.861***</t>
+  </si>
+  <si>
+    <t>-0.563*</t>
+  </si>
+  <si>
+    <t>-0.569*</t>
+  </si>
+  <si>
+    <t>-0.589**</t>
+  </si>
+  <si>
+    <t>Banks</t>
+  </si>
+  <si>
+    <t>Executive Branch</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>Judges and the Judiciary</t>
+  </si>
+  <si>
+    <t>Legislative Branch</t>
+  </si>
+  <si>
+    <t>Economic Institutions</t>
+  </si>
+  <si>
+    <t>Government Institutions</t>
+  </si>
+  <si>
+    <t>common</t>
+  </si>
+  <si>
+    <t>Medicine, Science, and Education</t>
+  </si>
+  <si>
+    <t>Media and Information</t>
+  </si>
+  <si>
+    <t>Social and Community</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>SE</t>
   </si>
 </sst>
 </file>
@@ -434,8 +771,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.000_);\(0.000\)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000_);\(0.000\)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -494,7 +831,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -511,16 +848,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -859,7 +1202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{372EFE93-148B-0746-BC26-D1E62E34FB02}">
   <dimension ref="A1:F371"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A354" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C363" sqref="C363"/>
     </sheetView>
@@ -13101,34 +13444,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15" t="s">
+      <c r="M1" s="16"/>
+      <c r="N1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="15"/>
+      <c r="O1" s="16"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -13178,7 +13521,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>107</v>
       </c>
       <c r="B3" s="12">
@@ -13225,7 +13568,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="13">
         <v>-20.03708</v>
       </c>
@@ -13270,7 +13613,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>111</v>
       </c>
       <c r="B5" s="12">
@@ -13317,7 +13660,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="13">
         <v>-9.3523300000000003</v>
       </c>
@@ -13362,7 +13705,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>112</v>
       </c>
       <c r="B7" s="12">
@@ -13409,7 +13752,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="13">
         <v>-11.99727</v>
       </c>
@@ -13454,7 +13797,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>113</v>
       </c>
       <c r="B9" s="12">
@@ -13501,7 +13844,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="13">
         <v>-13.10656</v>
       </c>
@@ -13546,7 +13889,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>114</v>
       </c>
       <c r="B11" s="12">
@@ -13593,7 +13936,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="13">
         <v>-12.79922</v>
       </c>
@@ -13638,7 +13981,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>115</v>
       </c>
       <c r="B13" s="12">
@@ -13685,7 +14028,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="13">
         <v>-4.1989900000000002</v>
       </c>
@@ -13730,7 +14073,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>116</v>
       </c>
       <c r="B15" s="12">
@@ -13777,7 +14120,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="13">
         <v>-15.262639999999999</v>
       </c>
@@ -13822,7 +14165,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="15" t="s">
         <v>117</v>
       </c>
       <c r="B17" s="12">
@@ -13869,7 +14212,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="13">
         <v>-7.3558399999999997</v>
       </c>
@@ -13914,7 +14257,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>118</v>
       </c>
       <c r="B19" s="12">
@@ -13961,7 +14304,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="13">
         <v>-18.034500000000001</v>
       </c>
@@ -14006,7 +14349,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="15" t="s">
         <v>119</v>
       </c>
       <c r="B21" s="12">
@@ -14053,7 +14396,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="16"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="13">
         <v>-12.1137</v>
       </c>
@@ -14098,7 +14441,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="15" t="s">
         <v>120</v>
       </c>
       <c r="B23" s="12">
@@ -14145,7 +14488,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="13">
         <v>-10.876958123</v>
       </c>
@@ -14190,7 +14533,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="15" t="s">
         <v>121</v>
       </c>
       <c r="B25" s="12">
@@ -14237,7 +14580,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="13">
         <v>-13.952842759999999</v>
       </c>
@@ -14282,7 +14625,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="15" t="s">
         <v>122</v>
       </c>
       <c r="B27" s="12">
@@ -14329,7 +14672,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="16"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="13">
         <v>-14.560277536999999</v>
       </c>
@@ -14374,7 +14717,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="15" t="s">
         <v>123</v>
       </c>
       <c r="B29" s="12">
@@ -14421,7 +14764,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="16"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="13">
         <v>-7.8518400000000002</v>
       </c>
@@ -14477,4 +14820,2964 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A721C35-D6D0-A64C-A700-8139672822CD}">
+  <dimension ref="A1:AI32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:O32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.83203125" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="1.83203125" customWidth="1"/>
+    <col min="17" max="17" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="1.83203125" customWidth="1"/>
+    <col min="28" max="28" width="1.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B1" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="H1" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="Q1" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AC1" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B2" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="14"/>
+      <c r="H2" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="O2" s="16"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="V2" s="16"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="14"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B3" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="H3" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="17">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C4" s="18">
+        <v>0.99952334545338495</v>
+      </c>
+      <c r="D4" s="17">
+        <v>1.141</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.992483554269594</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="18">
+        <v>0.96659960120729305</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="K4" s="18">
+        <v>0.985498588604794</v>
+      </c>
+      <c r="L4" s="17">
+        <v>0.255</v>
+      </c>
+      <c r="M4" s="18">
+        <v>0.99790693790839702</v>
+      </c>
+      <c r="N4" s="17">
+        <v>0.183</v>
+      </c>
+      <c r="O4" s="18">
+        <v>0.99875730824520703</v>
+      </c>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="R4" s="18">
+        <v>0.98847605730810095</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="T4" s="18">
+        <v>0.98807706767311099</v>
+      </c>
+      <c r="U4" s="17">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="V4" s="18">
+        <v>0.99343304445467795</v>
+      </c>
+      <c r="W4" s="18"/>
+      <c r="X4" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="Y4" s="18">
+        <v>0.98232383932672296</v>
+      </c>
+      <c r="Z4" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="AA4" s="18">
+        <v>0.98907071670415803</v>
+      </c>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17">
+        <v>0.109</v>
+      </c>
+      <c r="AD4" s="18">
+        <v>0.99928416707602996</v>
+      </c>
+      <c r="AE4" s="17">
+        <v>7.8E-2</v>
+      </c>
+      <c r="AF4" s="18">
+        <v>0.99949153772298904</v>
+      </c>
+      <c r="AG4" s="17">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="AH4" s="18">
+        <v>0.99872790075164697</v>
+      </c>
+      <c r="AI4" s="17"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="17">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="C5" s="18">
+        <v>5.1238883296719901</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="E5" s="18">
+        <v>5.1131207986170102</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="17">
+        <v>1.639</v>
+      </c>
+      <c r="I5" s="18">
+        <v>5.0922383917746901</v>
+      </c>
+      <c r="J5" s="17">
+        <v>3.0110000000000001</v>
+      </c>
+      <c r="K5" s="18">
+        <v>4.9983084747084296</v>
+      </c>
+      <c r="L5" s="17">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="M5" s="18">
+        <v>5.1018818904992704</v>
+      </c>
+      <c r="N5" s="17">
+        <v>3.9E-2</v>
+      </c>
+      <c r="O5" s="18">
+        <v>5.1267521579390296</v>
+      </c>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="17">
+        <v>1.0609999999999999</v>
+      </c>
+      <c r="R5" s="18">
+        <v>5.1116110032263</v>
+      </c>
+      <c r="S5" s="17">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="T5" s="18">
+        <v>5.10944911799817</v>
+      </c>
+      <c r="U5" s="17">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="V5" s="18">
+        <v>5.1049948624008197</v>
+      </c>
+      <c r="W5" s="18"/>
+      <c r="X5" s="17">
+        <v>2.8149999999999999</v>
+      </c>
+      <c r="Y5" s="18">
+        <v>5.0479451246059304</v>
+      </c>
+      <c r="Z5" s="17">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="AA5" s="18">
+        <v>5.0824968743702401</v>
+      </c>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="AD5" s="18">
+        <v>5.1252559093313401</v>
+      </c>
+      <c r="AE5" s="17">
+        <v>4.7E-2</v>
+      </c>
+      <c r="AF5" s="18">
+        <v>5.1259890117714804</v>
+      </c>
+      <c r="AG5" s="17">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="AH5" s="18">
+        <v>5.1168509176403303</v>
+      </c>
+      <c r="AI5" s="17"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="17">
+        <v>-0.01</v>
+      </c>
+      <c r="C6" s="18">
+        <v>5.1269102068891703</v>
+      </c>
+      <c r="D6" s="17">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="E6" s="18">
+        <v>5.1247316426848597</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="I6" s="18">
+        <v>5.1175164341752302</v>
+      </c>
+      <c r="J6" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="K6" s="18">
+        <v>5.0843003010150296</v>
+      </c>
+      <c r="L6" s="17">
+        <v>2E-3</v>
+      </c>
+      <c r="M6" s="18">
+        <v>5.1262270390986604</v>
+      </c>
+      <c r="N6" s="17">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="O6" s="18">
+        <v>5.1278332360637702</v>
+      </c>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="17">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="R6" s="18">
+        <v>5.1198392496837704</v>
+      </c>
+      <c r="S6" s="17">
+        <v>0.155</v>
+      </c>
+      <c r="T6" s="18">
+        <v>5.1238002830721801</v>
+      </c>
+      <c r="U6" s="17">
+        <v>-3.6999999999999998E-2</v>
+      </c>
+      <c r="V6" s="18">
+        <v>5.1205266316903302</v>
+      </c>
+      <c r="W6" s="18"/>
+      <c r="X6" s="17">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="Y6" s="18">
+        <v>5.1039579828078603</v>
+      </c>
+      <c r="Z6" s="17">
+        <v>-6.6000000000000003E-2</v>
+      </c>
+      <c r="AA6" s="18">
+        <v>5.1132012214526901</v>
+      </c>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AD6" s="18">
+        <v>5.1272299355340802</v>
+      </c>
+      <c r="AE6" s="17">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="AF6" s="18">
+        <v>5.12753534702503</v>
+      </c>
+      <c r="AG6" s="17">
+        <v>-1.7999999999999999E-2</v>
+      </c>
+      <c r="AH6" s="18">
+        <v>5.1261749219114296</v>
+      </c>
+      <c r="AI6" s="17"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="17">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="C7" s="18">
+        <v>5.1238883916507802</v>
+      </c>
+      <c r="D7" s="17">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E7" s="18">
+        <v>5.1132820773940999</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="17">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="I7" s="18">
+        <v>5.0927178392198904</v>
+      </c>
+      <c r="J7" s="17">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="K7" s="18">
+        <v>4.9983110522370202</v>
+      </c>
+      <c r="L7" s="17">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="M7" s="18">
+        <v>5.1018918011586898</v>
+      </c>
+      <c r="N7" s="17">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="O7" s="18">
+        <v>5.1267690512390596</v>
+      </c>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="17">
+        <v>0.49</v>
+      </c>
+      <c r="R7" s="18">
+        <v>5.1116949616167604</v>
+      </c>
+      <c r="S7" s="17">
+        <v>0.156</v>
+      </c>
+      <c r="T7" s="18">
+        <v>5.1096743122959802</v>
+      </c>
+      <c r="U7" s="17">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="V7" s="18">
+        <v>5.1050754562927203</v>
+      </c>
+      <c r="W7" s="18"/>
+      <c r="X7" s="17">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="Y7" s="18">
+        <v>5.0480187198895301</v>
+      </c>
+      <c r="Z7" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="AA7" s="18">
+        <v>5.0825469349061096</v>
+      </c>
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="17">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="AD7" s="18">
+        <v>5.1252661927921697</v>
+      </c>
+      <c r="AE7" s="17">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="AF7" s="18">
+        <v>5.1259945131249696</v>
+      </c>
+      <c r="AG7" s="17">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="AH7" s="18">
+        <v>5.1168567735851402</v>
+      </c>
+      <c r="AI7" s="17"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C8" s="18">
+        <v>5.1238883296719901</v>
+      </c>
+      <c r="D8" s="17">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="E8" s="18">
+        <v>5.1131207986170102</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="17">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="I8" s="18">
+        <v>5.0922383917746803</v>
+      </c>
+      <c r="J8" s="17">
+        <v>1.27</v>
+      </c>
+      <c r="K8" s="18">
+        <v>4.9983084747084296</v>
+      </c>
+      <c r="L8" s="17">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="M8" s="18">
+        <v>5.1018818904992704</v>
+      </c>
+      <c r="N8" s="17">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="O8" s="18">
+        <v>5.1267521579390296</v>
+      </c>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="17">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="R8" s="18">
+        <v>5.1116110032263</v>
+      </c>
+      <c r="S8" s="17">
+        <v>0.39</v>
+      </c>
+      <c r="T8" s="18">
+        <v>5.10944911799817</v>
+      </c>
+      <c r="U8" s="17">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="V8" s="18">
+        <v>5.1049948624008197</v>
+      </c>
+      <c r="W8" s="18"/>
+      <c r="X8" s="17">
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="Y8" s="18">
+        <v>5.0479451246059304</v>
+      </c>
+      <c r="Z8" s="17">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="AA8" s="18">
+        <v>5.0824968743702401</v>
+      </c>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AD8" s="18">
+        <v>5.1252559093313401</v>
+      </c>
+      <c r="AE8" s="17">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="AF8" s="18">
+        <v>5.1259890117714804</v>
+      </c>
+      <c r="AG8" s="17">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AH8" s="18">
+        <v>5.1168509176403303</v>
+      </c>
+      <c r="AI8" s="17"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="17">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C9" s="18">
+        <v>5.1238883296719901</v>
+      </c>
+      <c r="D9" s="17">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="E9" s="18">
+        <v>5.1131207986170102</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="17">
+        <v>1.415</v>
+      </c>
+      <c r="I9" s="18">
+        <v>5.0922383917746803</v>
+      </c>
+      <c r="J9" s="17">
+        <v>2.3559999999999999</v>
+      </c>
+      <c r="K9" s="18">
+        <v>4.9983084747084296</v>
+      </c>
+      <c r="L9" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="M9" s="18">
+        <v>5.1018818904992704</v>
+      </c>
+      <c r="N9" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="O9" s="18">
+        <v>5.1267521579390296</v>
+      </c>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="17">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="R9" s="18">
+        <v>5.1116110032263</v>
+      </c>
+      <c r="S9" s="17">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="T9" s="18">
+        <v>5.10944911799817</v>
+      </c>
+      <c r="U9" s="17">
+        <v>0.443</v>
+      </c>
+      <c r="V9" s="18">
+        <v>5.1049948624008197</v>
+      </c>
+      <c r="W9" s="18"/>
+      <c r="X9" s="17">
+        <v>2.3580000000000001</v>
+      </c>
+      <c r="Y9" s="18">
+        <v>5.0479451246059304</v>
+      </c>
+      <c r="Z9" s="17">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="AA9" s="18">
+        <v>5.0824968743702401</v>
+      </c>
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="17">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AD9" s="18">
+        <v>5.1252559093313401</v>
+      </c>
+      <c r="AE9" s="17">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AF9" s="18">
+        <v>5.1259890117714804</v>
+      </c>
+      <c r="AG9" s="17">
+        <v>0.193</v>
+      </c>
+      <c r="AH9" s="18">
+        <v>5.1168509176403303</v>
+      </c>
+      <c r="AI9" s="17"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="17">
+        <v>-1.9E-2</v>
+      </c>
+      <c r="C10" s="18">
+        <v>5.1265925087044</v>
+      </c>
+      <c r="D10" s="17">
+        <v>2E-3</v>
+      </c>
+      <c r="E10" s="18">
+        <v>5.1146191280763098</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="17">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="I10" s="18">
+        <v>5.1086181718023402</v>
+      </c>
+      <c r="J10" s="17">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="K10" s="18">
+        <v>5.0333230589658102</v>
+      </c>
+      <c r="L10" s="17">
+        <v>-2.8000000000000001E-2</v>
+      </c>
+      <c r="M10" s="18">
+        <v>5.1239209073175997</v>
+      </c>
+      <c r="N10" s="17">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="O10" s="18">
+        <v>5.1270676543098999</v>
+      </c>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="17">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="R10" s="18">
+        <v>5.1144172463905999</v>
+      </c>
+      <c r="S10" s="17">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="T10" s="18">
+        <v>5.1182196849059203</v>
+      </c>
+      <c r="U10" s="17">
+        <v>-0.223</v>
+      </c>
+      <c r="V10" s="18">
+        <v>5.1071061681665704</v>
+      </c>
+      <c r="W10" s="18"/>
+      <c r="X10" s="17">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="Y10" s="18">
+        <v>5.0856875516927502</v>
+      </c>
+      <c r="Z10" s="17">
+        <v>-0.13200000000000001</v>
+      </c>
+      <c r="AA10" s="18">
+        <v>5.0841023697583303</v>
+      </c>
+      <c r="AB10" s="17"/>
+      <c r="AC10" s="17">
+        <v>-1.4E-2</v>
+      </c>
+      <c r="AD10" s="18">
+        <v>5.12682591675763</v>
+      </c>
+      <c r="AE10" s="17">
+        <v>-1.4999999999999999E-2</v>
+      </c>
+      <c r="AF10" s="18">
+        <v>5.1273595322919503</v>
+      </c>
+      <c r="AG10" s="17">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="AH10" s="18">
+        <v>5.1168509537261002</v>
+      </c>
+      <c r="AI10" s="17"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="17">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="C11" s="18">
+        <v>5.1238883296719901</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="E11" s="18">
+        <v>5.1131207986170102</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="17">
+        <v>1.5349999999999999</v>
+      </c>
+      <c r="I11" s="18">
+        <v>5.0922383917746803</v>
+      </c>
+      <c r="J11" s="17">
+        <v>3.0219999999999998</v>
+      </c>
+      <c r="K11" s="18">
+        <v>4.9983084747084296</v>
+      </c>
+      <c r="L11" s="17">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="M11" s="18">
+        <v>5.1018818904992704</v>
+      </c>
+      <c r="N11" s="17">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="O11" s="18">
+        <v>5.1267521579390296</v>
+      </c>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="17">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="R11" s="18">
+        <v>5.1116110032263</v>
+      </c>
+      <c r="S11" s="17">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="T11" s="18">
+        <v>5.10944911799817</v>
+      </c>
+      <c r="U11" s="17">
+        <v>0.496</v>
+      </c>
+      <c r="V11" s="18">
+        <v>5.1049948624008197</v>
+      </c>
+      <c r="W11" s="18"/>
+      <c r="X11" s="17">
+        <v>2.5960000000000001</v>
+      </c>
+      <c r="Y11" s="18">
+        <v>5.0479451246059304</v>
+      </c>
+      <c r="Z11" s="17">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="AA11" s="18">
+        <v>5.0824968743702401</v>
+      </c>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="AD11" s="18">
+        <v>5.1252559093313401</v>
+      </c>
+      <c r="AE11" s="17">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="AF11" s="18">
+        <v>5.1259890117714804</v>
+      </c>
+      <c r="AG11" s="17">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="AH11" s="18">
+        <v>5.1168509176403303</v>
+      </c>
+      <c r="AI11" s="17"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="17">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="C12" s="18">
+        <v>5.1238883296719901</v>
+      </c>
+      <c r="D12" s="17">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="E12" s="18">
+        <v>5.1131207986170102</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" t="s">
+        <v>124</v>
+      </c>
+      <c r="H12" s="17">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="I12" s="18">
+        <v>5.0922383917746803</v>
+      </c>
+      <c r="J12" s="17">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="K12" s="18">
+        <v>4.9983084747084296</v>
+      </c>
+      <c r="L12" s="17">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="M12" s="18">
+        <v>5.1018818904992704</v>
+      </c>
+      <c r="N12" s="17">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="O12" s="18">
+        <v>5.1267521579390296</v>
+      </c>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="17">
+        <v>0.72</v>
+      </c>
+      <c r="R12" s="18">
+        <v>5.1116110032263</v>
+      </c>
+      <c r="S12" s="17">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="T12" s="18">
+        <v>5.10944911799817</v>
+      </c>
+      <c r="U12" s="17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="V12" s="18">
+        <v>5.1049948624008197</v>
+      </c>
+      <c r="W12" s="18"/>
+      <c r="X12" s="17">
+        <v>1.2989999999999999</v>
+      </c>
+      <c r="Y12" s="18">
+        <v>5.0479451246059304</v>
+      </c>
+      <c r="Z12" s="17">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AA12" s="18">
+        <v>5.0824968743702401</v>
+      </c>
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AD12" s="18">
+        <v>5.1252559093313401</v>
+      </c>
+      <c r="AE12" s="17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AF12" s="18">
+        <v>5.1259890117714804</v>
+      </c>
+      <c r="AG12" s="17">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="AH12" s="18">
+        <v>5.1168509176403303</v>
+      </c>
+      <c r="AI12" s="17"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="17">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C13" s="18">
+        <v>5.1238883296719901</v>
+      </c>
+      <c r="D13" s="17">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="E13" s="18">
+        <v>5.1131207986170102</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="17">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="I13" s="18">
+        <v>5.0922383917746803</v>
+      </c>
+      <c r="J13" s="17">
+        <v>1.385</v>
+      </c>
+      <c r="K13" s="18">
+        <v>4.9983084747084296</v>
+      </c>
+      <c r="L13" s="17">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="M13" s="18">
+        <v>5.1018818904992704</v>
+      </c>
+      <c r="N13" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="O13" s="18">
+        <v>5.1267521579390296</v>
+      </c>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="17">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="R13" s="18">
+        <v>5.1116110032263</v>
+      </c>
+      <c r="S13" s="17">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="T13" s="18">
+        <v>5.10944911799817</v>
+      </c>
+      <c r="U13" s="17">
+        <v>0.223</v>
+      </c>
+      <c r="V13" s="18">
+        <v>5.1049948624008197</v>
+      </c>
+      <c r="W13" s="18"/>
+      <c r="X13" s="17">
+        <v>1.22</v>
+      </c>
+      <c r="Y13" s="18">
+        <v>5.0479451246059304</v>
+      </c>
+      <c r="Z13" s="17">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="AA13" s="18">
+        <v>5.0824968743702401</v>
+      </c>
+      <c r="AB13" s="17"/>
+      <c r="AC13" s="17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AD13" s="18">
+        <v>5.1252559093313401</v>
+      </c>
+      <c r="AE13" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AF13" s="18">
+        <v>5.1259890117714804</v>
+      </c>
+      <c r="AG13" s="17">
+        <v>0.112</v>
+      </c>
+      <c r="AH13" s="18">
+        <v>5.1168509176403303</v>
+      </c>
+      <c r="AI13" s="17"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="17">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="C14" s="18">
+        <v>5.1268908112387503</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0.11</v>
+      </c>
+      <c r="E14" s="18">
+        <v>5.1246608758283703</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="17">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="I14" s="18">
+        <v>5.1143752924547004</v>
+      </c>
+      <c r="J14" s="17">
+        <v>1.244</v>
+      </c>
+      <c r="K14" s="18">
+        <v>5.0781007307004504</v>
+      </c>
+      <c r="L14" s="17">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="M14" s="18">
+        <v>5.1259520807265204</v>
+      </c>
+      <c r="N14" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="O14" s="18">
+        <v>5.1278122078505604</v>
+      </c>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="R14" s="18">
+        <v>5.11679253118111</v>
+      </c>
+      <c r="S14" s="17">
+        <v>0.247</v>
+      </c>
+      <c r="T14" s="18">
+        <v>5.1227223584574402</v>
+      </c>
+      <c r="U14" s="17">
+        <v>1.4E-2</v>
+      </c>
+      <c r="V14" s="18">
+        <v>5.1203163029170504</v>
+      </c>
+      <c r="W14" s="18"/>
+      <c r="X14" s="17">
+        <v>0.432</v>
+      </c>
+      <c r="Y14" s="18">
+        <v>5.1008812167376698</v>
+      </c>
+      <c r="Z14" s="17">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AA14" s="18">
+        <v>5.1111759466029199</v>
+      </c>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AD14" s="18">
+        <v>5.1272140585622896</v>
+      </c>
+      <c r="AE14" s="17">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="AF14" s="18">
+        <v>5.1275316081108597</v>
+      </c>
+      <c r="AG14" s="17">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="AH14" s="18">
+        <v>5.1261645972367802</v>
+      </c>
+      <c r="AI14" s="17"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C15" s="18">
+        <v>5.12660369987836</v>
+      </c>
+      <c r="D15" s="17">
+        <v>0.161</v>
+      </c>
+      <c r="E15" s="18">
+        <v>5.1241942088624599</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="17">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="I15" s="18">
+        <v>5.1151238805506196</v>
+      </c>
+      <c r="J15" s="17">
+        <v>1.5049999999999999</v>
+      </c>
+      <c r="K15" s="18">
+        <v>5.0755308476847603</v>
+      </c>
+      <c r="L15" s="17">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="M15" s="18">
+        <v>5.1261042567496702</v>
+      </c>
+      <c r="N15" s="17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="O15" s="18">
+        <v>5.1278047227568297</v>
+      </c>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="17">
+        <v>0.309</v>
+      </c>
+      <c r="R15" s="18">
+        <v>5.1206105696522997</v>
+      </c>
+      <c r="S15" s="17">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="T15" s="18">
+        <v>5.1233767386080098</v>
+      </c>
+      <c r="U15" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="V15" s="18">
+        <v>5.1187866180692998</v>
+      </c>
+      <c r="W15" s="18"/>
+      <c r="X15" s="17">
+        <v>1.0429999999999999</v>
+      </c>
+      <c r="Y15" s="18">
+        <v>5.09689641939051</v>
+      </c>
+      <c r="Z15" s="17">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="AA15" s="18">
+        <v>5.0970016441179897</v>
+      </c>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17">
+        <v>1.9E-2</v>
+      </c>
+      <c r="AD15" s="18">
+        <v>5.1270266773745403</v>
+      </c>
+      <c r="AE15" s="17">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AF15" s="18">
+        <v>5.1274580439084003</v>
+      </c>
+      <c r="AG15" s="17">
+        <v>2.4E-2</v>
+      </c>
+      <c r="AH15" s="18">
+        <v>5.1256179062583502</v>
+      </c>
+      <c r="AI15" s="17"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="17">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="C16" s="18">
+        <v>5.1238883296719901</v>
+      </c>
+      <c r="D16" s="17">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="E16" s="18">
+        <v>5.1131207986170102</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="17">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="I16" s="18">
+        <v>5.0922383917746803</v>
+      </c>
+      <c r="J16" s="17">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="K16" s="18">
+        <v>4.9983084747084296</v>
+      </c>
+      <c r="L16" s="17">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="M16" s="18">
+        <v>5.1018818904992704</v>
+      </c>
+      <c r="N16" s="17">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="O16" s="18">
+        <v>5.1267521579390296</v>
+      </c>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="17">
+        <v>0.747</v>
+      </c>
+      <c r="R16" s="18">
+        <v>5.1116110032263</v>
+      </c>
+      <c r="S16" s="17">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="T16" s="18">
+        <v>5.10944911799817</v>
+      </c>
+      <c r="U16" s="17">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="V16" s="18">
+        <v>5.1049948624008197</v>
+      </c>
+      <c r="W16" s="18"/>
+      <c r="X16" s="17">
+        <v>1.589</v>
+      </c>
+      <c r="Y16" s="18">
+        <v>5.0479451246059304</v>
+      </c>
+      <c r="Z16" s="17">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="AA16" s="18">
+        <v>5.0824968743702401</v>
+      </c>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17">
+        <v>2.7E-2</v>
+      </c>
+      <c r="AD16" s="18">
+        <v>5.1252559093313401</v>
+      </c>
+      <c r="AE16" s="17">
+        <v>1.9E-2</v>
+      </c>
+      <c r="AF16" s="18">
+        <v>5.1259890117714804</v>
+      </c>
+      <c r="AG16" s="17">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AH16" s="18">
+        <v>5.1168509176403303</v>
+      </c>
+      <c r="AI16" s="17"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C17" s="18">
+        <v>5.1238885122004501</v>
+      </c>
+      <c r="D17" s="17">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="E17" s="18">
+        <v>5.1132532991320803</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="17">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="I17" s="18">
+        <v>5.0926812617629498</v>
+      </c>
+      <c r="J17" s="17">
+        <v>1.3360000000000001</v>
+      </c>
+      <c r="K17" s="18">
+        <v>4.99831032277765</v>
+      </c>
+      <c r="L17" s="17">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="M17" s="18">
+        <v>5.1018831367203399</v>
+      </c>
+      <c r="N17" s="17">
+        <v>-1E-3</v>
+      </c>
+      <c r="O17" s="18">
+        <v>5.1267690801313801</v>
+      </c>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="17">
+        <v>1.0529999999999999</v>
+      </c>
+      <c r="R17" s="18">
+        <v>5.1116644885321998</v>
+      </c>
+      <c r="S17" s="17">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="T17" s="18">
+        <v>5.1096734705632496</v>
+      </c>
+      <c r="U17" s="17">
+        <v>-7.8E-2</v>
+      </c>
+      <c r="V17" s="18">
+        <v>5.1050642181803498</v>
+      </c>
+      <c r="W17" s="18"/>
+      <c r="X17" s="17">
+        <v>1.278</v>
+      </c>
+      <c r="Y17" s="18">
+        <v>5.0479496522086098</v>
+      </c>
+      <c r="Z17" s="17">
+        <v>-0.32</v>
+      </c>
+      <c r="AA17" s="18">
+        <v>5.0825412051479404</v>
+      </c>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17">
+        <v>2.3E-2</v>
+      </c>
+      <c r="AD17" s="18">
+        <v>5.1252662831923104</v>
+      </c>
+      <c r="AE17" s="17">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AF17" s="18">
+        <v>5.1259936433081004</v>
+      </c>
+      <c r="AG17" s="17">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AH17" s="18">
+        <v>5.1168538315835796</v>
+      </c>
+      <c r="AI17" s="17"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="18"/>
+      <c r="W18" s="18"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="18"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="18"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="18"/>
+      <c r="AE18" s="17"/>
+      <c r="AF18" s="18"/>
+      <c r="AG18" s="17"/>
+      <c r="AH18" s="18"/>
+      <c r="AI18" s="17"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>235</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="18">
+        <v>0.275979078964953</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="18">
+        <v>0.27681887230858998</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" t="s">
+        <v>235</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="I19" s="18">
+        <v>0.282018627772604</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="K19" s="18">
+        <v>0.28412173241572902</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="M19" s="18">
+        <v>0.27603122514773898</v>
+      </c>
+      <c r="N19" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="O19" s="18">
+        <v>0.27552859696938098</v>
+      </c>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="R19" s="18">
+        <v>0.27654208872096397</v>
+      </c>
+      <c r="S19" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="T19" s="18">
+        <v>0.27682166166664102</v>
+      </c>
+      <c r="U19" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="V19" s="18">
+        <v>0.28322289472177697</v>
+      </c>
+      <c r="W19" s="18"/>
+      <c r="X19" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="Y19" s="18">
+        <v>0.29084411986415099</v>
+      </c>
+      <c r="Z19" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="AA19" s="18">
+        <v>0.29044970933969499</v>
+      </c>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD19" s="18">
+        <v>0.27544081052679498</v>
+      </c>
+      <c r="AE19" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF19" s="18">
+        <v>0.27543753407127403</v>
+      </c>
+      <c r="AG19" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="AH19" s="18">
+        <v>0.27690858065179202</v>
+      </c>
+      <c r="AI19" s="17"/>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="18">
+        <v>0.34436126358876501</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E20" s="18">
+        <v>0.45186546121746501</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="I20" s="18">
+        <v>0.56838434992184295</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="K20" s="18">
+        <v>1.0992183888977201</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="M20" s="18">
+        <v>0.42598404042715599</v>
+      </c>
+      <c r="N20" s="17">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="O20" s="18">
+        <v>0.29885451080228997</v>
+      </c>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="R20" s="18">
+        <v>0.41735974694905698</v>
+      </c>
+      <c r="S20" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="T20" s="18">
+        <v>0.46197139815357302</v>
+      </c>
+      <c r="U20" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="V20" s="18">
+        <v>0.469385575674234</v>
+      </c>
+      <c r="W20" s="18"/>
+      <c r="X20" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y20" s="18">
+        <v>0.653110283906572</v>
+      </c>
+      <c r="Z20" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="AA20" s="18">
+        <v>0.70303119687451499</v>
+      </c>
+      <c r="AB20" s="17"/>
+      <c r="AC20" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="AD20" s="18">
+        <v>0.31605038655220002</v>
+      </c>
+      <c r="AE20" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF20" s="18">
+        <v>0.30372352545264297</v>
+      </c>
+      <c r="AG20" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="AH20" s="18">
+        <v>0.39702329086695698</v>
+      </c>
+      <c r="AI20" s="17"/>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="17">
+        <v>-0.37</v>
+      </c>
+      <c r="C21" s="18">
+        <v>3.4338289107053099</v>
+      </c>
+      <c r="D21" s="17">
+        <v>-1.7000000000000001E-2</v>
+      </c>
+      <c r="E21" s="18">
+        <v>3.4370543495410302</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="17">
+        <v>-0.79900000000000004</v>
+      </c>
+      <c r="I21" s="18">
+        <v>3.4456793932435299</v>
+      </c>
+      <c r="J21" s="17">
+        <v>3.0950000000000002</v>
+      </c>
+      <c r="K21" s="18">
+        <v>3.49613161851084</v>
+      </c>
+      <c r="L21" s="17">
+        <v>-9.2999999999999999E-2</v>
+      </c>
+      <c r="M21" s="18">
+        <v>3.4348502978909399</v>
+      </c>
+      <c r="N21" s="17">
+        <v>-0.70299999999999996</v>
+      </c>
+      <c r="O21" s="18">
+        <v>3.4323269714274498</v>
+      </c>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="17">
+        <v>1.107</v>
+      </c>
+      <c r="R21" s="18">
+        <v>3.4428198476820202</v>
+      </c>
+      <c r="S21" s="17">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="T21" s="18">
+        <v>3.43839912752322</v>
+      </c>
+      <c r="U21" s="17">
+        <v>-1.218</v>
+      </c>
+      <c r="V21" s="18">
+        <v>3.44340178967609</v>
+      </c>
+      <c r="W21" s="18"/>
+      <c r="X21" s="17">
+        <v>-0.35399999999999998</v>
+      </c>
+      <c r="Y21" s="18">
+        <v>3.4691700097781601</v>
+      </c>
+      <c r="Z21" s="17">
+        <v>-1.5</v>
+      </c>
+      <c r="AA21" s="18">
+        <v>3.45525884416364</v>
+      </c>
+      <c r="AB21" s="17"/>
+      <c r="AC21" s="17">
+        <v>-0.158</v>
+      </c>
+      <c r="AD21" s="18">
+        <v>3.4332927176108599</v>
+      </c>
+      <c r="AE21" s="17">
+        <v>-0.35599999999999998</v>
+      </c>
+      <c r="AF21" s="18">
+        <v>3.43282416955714</v>
+      </c>
+      <c r="AG21" s="17">
+        <v>-0.56699999999999995</v>
+      </c>
+      <c r="AH21" s="18">
+        <v>3.4349666543427202</v>
+      </c>
+      <c r="AI21" s="17"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="17">
+        <v>-0.53900000000000003</v>
+      </c>
+      <c r="C22" s="18">
+        <v>0.34436374907609202</v>
+      </c>
+      <c r="D22" s="17">
+        <v>-4.4999999999999998E-2</v>
+      </c>
+      <c r="E22" s="18">
+        <v>0.45179890525752298</v>
+      </c>
+      <c r="F22" s="18"/>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="I22" s="18">
+        <v>0.56875127959812399</v>
+      </c>
+      <c r="J22" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="K22" s="18">
+        <v>1.0993261567022801</v>
+      </c>
+      <c r="L22" s="17">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="M22" s="18">
+        <v>0.42596200618492402</v>
+      </c>
+      <c r="N22" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="O22" s="18">
+        <v>0.298896090529845</v>
+      </c>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="17">
+        <v>-0.248</v>
+      </c>
+      <c r="R22" s="18">
+        <v>0.417359242354856</v>
+      </c>
+      <c r="S22" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="T22" s="18">
+        <v>0.46176845853501203</v>
+      </c>
+      <c r="U22" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="V22" s="18">
+        <v>0.46934067378744498</v>
+      </c>
+      <c r="W22" s="18"/>
+      <c r="X22" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y22" s="18">
+        <v>0.65293258689524303</v>
+      </c>
+      <c r="Z22" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="AA22" s="18">
+        <v>0.70301048037237401</v>
+      </c>
+      <c r="AB22" s="17"/>
+      <c r="AC22" s="17">
+        <v>-0.47899999999999998</v>
+      </c>
+      <c r="AD22" s="18">
+        <v>0.31602047038251002</v>
+      </c>
+      <c r="AE22" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF22" s="18">
+        <v>0.30371861022185098</v>
+      </c>
+      <c r="AG22" s="17">
+        <v>-0.55500000000000005</v>
+      </c>
+      <c r="AH22" s="18">
+        <v>0.397040735090821</v>
+      </c>
+      <c r="AI22" s="17"/>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="17">
+        <v>-0.17</v>
+      </c>
+      <c r="C23" s="18">
+        <v>0.34436126358876201</v>
+      </c>
+      <c r="D23" s="17">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="E23" s="18">
+        <v>0.45186546121746601</v>
+      </c>
+      <c r="F23" s="18"/>
+      <c r="G23" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="17">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="I23" s="18">
+        <v>0.56838434992184195</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="K23" s="18">
+        <v>1.0992183888977201</v>
+      </c>
+      <c r="L23" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="M23" s="18">
+        <v>0.42598404042715599</v>
+      </c>
+      <c r="N23" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="O23" s="18">
+        <v>0.29885451080228997</v>
+      </c>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="17">
+        <v>0.308</v>
+      </c>
+      <c r="R23" s="18">
+        <v>0.41735974694905598</v>
+      </c>
+      <c r="S23" s="17">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="T23" s="18">
+        <v>0.46197139815357402</v>
+      </c>
+      <c r="U23" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="V23" s="18">
+        <v>0.469385575674234</v>
+      </c>
+      <c r="W23" s="18"/>
+      <c r="X23" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y23" s="18">
+        <v>0.653110283906572</v>
+      </c>
+      <c r="Z23" s="17">
+        <v>-1.0860000000000001</v>
+      </c>
+      <c r="AA23" s="18">
+        <v>0.70303119687451499</v>
+      </c>
+      <c r="AB23" s="17"/>
+      <c r="AC23" s="17">
+        <v>-0.20200000000000001</v>
+      </c>
+      <c r="AD23" s="18">
+        <v>0.31605038655219803</v>
+      </c>
+      <c r="AE23" s="17">
+        <v>-0.43</v>
+      </c>
+      <c r="AF23" s="18">
+        <v>0.30372352545264197</v>
+      </c>
+      <c r="AG23" s="17">
+        <v>-4.5999999999999999E-2</v>
+      </c>
+      <c r="AH23" s="18">
+        <v>0.39702329086695498</v>
+      </c>
+      <c r="AI23" s="17"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="18">
+        <v>0.34436126358876201</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E24" s="18">
+        <v>0.45186546121746601</v>
+      </c>
+      <c r="F24" s="18"/>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="I24" s="18">
+        <v>0.56838434992184195</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="K24" s="18">
+        <v>1.0992183888977201</v>
+      </c>
+      <c r="L24" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="M24" s="18">
+        <v>0.42598404042715698</v>
+      </c>
+      <c r="N24" s="17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="O24" s="18">
+        <v>0.29885451080228997</v>
+      </c>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="R24" s="18">
+        <v>0.41735974694905598</v>
+      </c>
+      <c r="S24" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="T24" s="18">
+        <v>0.46197139815357402</v>
+      </c>
+      <c r="U24" s="17">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="V24" s="18">
+        <v>0.469385575674233</v>
+      </c>
+      <c r="W24" s="18"/>
+      <c r="X24" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="Y24" s="18">
+        <v>0.653110283906571</v>
+      </c>
+      <c r="Z24" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA24" s="18">
+        <v>0.70303119687451499</v>
+      </c>
+      <c r="AB24" s="17"/>
+      <c r="AC24" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="AD24" s="18">
+        <v>0.31605038655219903</v>
+      </c>
+      <c r="AE24" s="17">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="AF24" s="18">
+        <v>0.30372352545264197</v>
+      </c>
+      <c r="AG24" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="AH24" s="18">
+        <v>0.39702329086695498</v>
+      </c>
+      <c r="AI24" s="17"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="17">
+        <v>-0.621</v>
+      </c>
+      <c r="C25" s="18">
+        <v>2.87996429321942</v>
+      </c>
+      <c r="D25" s="17">
+        <v>-1.0309999999999999</v>
+      </c>
+      <c r="E25" s="18">
+        <v>1.5456829382281301</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="I25" s="18">
+        <v>1.5592140463500199</v>
+      </c>
+      <c r="J25" s="17">
+        <v>-1.2330000000000001</v>
+      </c>
+      <c r="K25" s="18">
+        <v>1.77276831100979</v>
+      </c>
+      <c r="L25" s="17">
+        <v>-1.161</v>
+      </c>
+      <c r="M25" s="18">
+        <v>1.5208019713632701</v>
+      </c>
+      <c r="N25" s="17">
+        <v>-1.179</v>
+      </c>
+      <c r="O25" s="18">
+        <v>1.51215607824819</v>
+      </c>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="17">
+        <v>-1.1839999999999999</v>
+      </c>
+      <c r="R25" s="18">
+        <v>1.53354593233976</v>
+      </c>
+      <c r="S25" s="17">
+        <v>-1.22</v>
+      </c>
+      <c r="T25" s="18">
+        <v>1.53717544621165</v>
+      </c>
+      <c r="U25" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="V25" s="18">
+        <v>1.57265355929517</v>
+      </c>
+      <c r="W25" s="18"/>
+      <c r="X25" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y25" s="18">
+        <v>1.5686937832619701</v>
+      </c>
+      <c r="Z25" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA25" s="18">
+        <v>1.6378575393952199</v>
+      </c>
+      <c r="AB25" s="17"/>
+      <c r="AC25" s="17">
+        <v>-1.0089999999999999</v>
+      </c>
+      <c r="AD25" s="18">
+        <v>1.51356857574939</v>
+      </c>
+      <c r="AE25" s="17">
+        <v>-1.119</v>
+      </c>
+      <c r="AF25" s="18">
+        <v>1.51170501240162</v>
+      </c>
+      <c r="AG25" s="17">
+        <v>-1.2070000000000001</v>
+      </c>
+      <c r="AH25" s="18">
+        <v>1.5381078127278001</v>
+      </c>
+      <c r="AI25" s="17"/>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" s="18">
+        <v>0.34436126358876501</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="18">
+        <v>0.45186546121746601</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="I26" s="18">
+        <v>0.56838434992184195</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="K26" s="18">
+        <v>1.0992183888977201</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="M26" s="18">
+        <v>0.42598404042715698</v>
+      </c>
+      <c r="N26" s="17">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="O26" s="18">
+        <v>0.29885451080228997</v>
+      </c>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="R26" s="18">
+        <v>0.41735974694905698</v>
+      </c>
+      <c r="S26" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="T26" s="18">
+        <v>0.46197139815357302</v>
+      </c>
+      <c r="U26" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="V26" s="18">
+        <v>0.469385575674234</v>
+      </c>
+      <c r="W26" s="18"/>
+      <c r="X26" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y26" s="18">
+        <v>0.653110283906572</v>
+      </c>
+      <c r="Z26" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA26" s="18">
+        <v>0.70303119687451499</v>
+      </c>
+      <c r="AB26" s="17"/>
+      <c r="AC26" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD26" s="18">
+        <v>0.31605038655219903</v>
+      </c>
+      <c r="AE26" s="17">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="AF26" s="18">
+        <v>0.30372352545264197</v>
+      </c>
+      <c r="AG26" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="AH26" s="18">
+        <v>0.39702329086695498</v>
+      </c>
+      <c r="AI26" s="17"/>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="18">
+        <v>0.34436126358876501</v>
+      </c>
+      <c r="D27" s="17">
+        <v>-0.13900000000000001</v>
+      </c>
+      <c r="E27" s="18">
+        <v>0.45186546121746601</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" t="s">
+        <v>124</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I27" s="18">
+        <v>0.56838434992184195</v>
+      </c>
+      <c r="J27" s="17">
+        <v>1.6060000000000001</v>
+      </c>
+      <c r="K27" s="18">
+        <v>1.0992183888977201</v>
+      </c>
+      <c r="L27" s="17">
+        <v>0.123</v>
+      </c>
+      <c r="M27" s="18">
+        <v>0.42598404042715698</v>
+      </c>
+      <c r="N27" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="O27" s="18">
+        <v>0.29885451080228898</v>
+      </c>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="17">
+        <v>-0.34</v>
+      </c>
+      <c r="R27" s="18">
+        <v>0.41735974694905698</v>
+      </c>
+      <c r="S27" s="17">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="T27" s="18">
+        <v>0.46197139815357302</v>
+      </c>
+      <c r="U27" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="V27" s="18">
+        <v>0.469385575674233</v>
+      </c>
+      <c r="W27" s="18"/>
+      <c r="X27" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y27" s="18">
+        <v>0.653110283906572</v>
+      </c>
+      <c r="Z27" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA27" s="18">
+        <v>0.70303119687451499</v>
+      </c>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="17">
+        <v>-0.51900000000000002</v>
+      </c>
+      <c r="AD27" s="18">
+        <v>0.31605038655219803</v>
+      </c>
+      <c r="AE27" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="AF27" s="18">
+        <v>0.30372352545264197</v>
+      </c>
+      <c r="AG27" s="17">
+        <v>-0.624</v>
+      </c>
+      <c r="AH27" s="18">
+        <v>0.39702329086695498</v>
+      </c>
+      <c r="AI27" s="17"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="17">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="C28" s="18">
+        <v>0.34436126358876101</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E28" s="18">
+        <v>0.45186546121746601</v>
+      </c>
+      <c r="F28" s="18"/>
+      <c r="G28" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" s="17">
+        <v>-0.314</v>
+      </c>
+      <c r="I28" s="18">
+        <v>0.56838434992184195</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="K28" s="18">
+        <v>1.0992183888977201</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="M28" s="18">
+        <v>0.42598404042715698</v>
+      </c>
+      <c r="N28" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="O28" s="18">
+        <v>0.29885451080228898</v>
+      </c>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="17">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="R28" s="18">
+        <v>0.41735974694905698</v>
+      </c>
+      <c r="S28" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="T28" s="18">
+        <v>0.46197139815357302</v>
+      </c>
+      <c r="U28" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="V28" s="18">
+        <v>0.469385575674234</v>
+      </c>
+      <c r="W28" s="18"/>
+      <c r="X28" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="Y28" s="18">
+        <v>0.653110283906572</v>
+      </c>
+      <c r="Z28" s="17">
+        <v>-0.76700000000000002</v>
+      </c>
+      <c r="AA28" s="18">
+        <v>0.70303119687451399</v>
+      </c>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="17">
+        <v>-0.123</v>
+      </c>
+      <c r="AD28" s="18">
+        <v>0.31605038655219903</v>
+      </c>
+      <c r="AE28" s="17">
+        <v>-0.36499999999999999</v>
+      </c>
+      <c r="AF28" s="18">
+        <v>0.30372352545264197</v>
+      </c>
+      <c r="AG28" s="17">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AH28" s="18">
+        <v>0.39702329086695498</v>
+      </c>
+      <c r="AI28" s="17"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="17">
+        <v>-0.188</v>
+      </c>
+      <c r="C29" s="18">
+        <v>3.4338289082172802</v>
+      </c>
+      <c r="D29" s="17">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="E29" s="18">
+        <v>3.43705412191773</v>
+      </c>
+      <c r="F29" s="18"/>
+      <c r="G29" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" s="17">
+        <v>-0.375</v>
+      </c>
+      <c r="I29" s="18">
+        <v>3.4456552918509602</v>
+      </c>
+      <c r="J29" s="17">
+        <v>3.9790000000000001</v>
+      </c>
+      <c r="K29" s="18">
+        <v>3.4959259566913201</v>
+      </c>
+      <c r="L29" s="17">
+        <v>0.124</v>
+      </c>
+      <c r="M29" s="18">
+        <v>3.4348499610486498</v>
+      </c>
+      <c r="N29" s="17">
+        <v>-0.59599999999999997</v>
+      </c>
+      <c r="O29" s="18">
+        <v>3.43232696698808</v>
+      </c>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="17">
+        <v>1.478</v>
+      </c>
+      <c r="R29" s="18">
+        <v>3.4427894076648999</v>
+      </c>
+      <c r="S29" s="17">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="T29" s="18">
+        <v>3.4383932765235401</v>
+      </c>
+      <c r="U29" s="17">
+        <v>-0.80700000000000005</v>
+      </c>
+      <c r="V29" s="18">
+        <v>3.44340139526274</v>
+      </c>
+      <c r="W29" s="18"/>
+      <c r="X29" s="17">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="Y29" s="18">
+        <v>3.4691055619561699</v>
+      </c>
+      <c r="Z29" s="17">
+        <v>-0.93</v>
+      </c>
+      <c r="AA29" s="18">
+        <v>3.4552255204999098</v>
+      </c>
+      <c r="AB29" s="17"/>
+      <c r="AC29" s="17">
+        <v>1E-3</v>
+      </c>
+      <c r="AD29" s="18">
+        <v>3.4332926646450299</v>
+      </c>
+      <c r="AE29" s="17">
+        <v>-0.219</v>
+      </c>
+      <c r="AF29" s="18">
+        <v>3.4328241540856301</v>
+      </c>
+      <c r="AG29" s="17">
+        <v>-0.34499999999999997</v>
+      </c>
+      <c r="AH29" s="18">
+        <v>3.4349666279730098</v>
+      </c>
+      <c r="AI29" s="17"/>
+    </row>
+    <row r="30" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="17">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="C30" s="18">
+        <v>2.8799643132257602</v>
+      </c>
+      <c r="D30" s="17">
+        <v>1.139</v>
+      </c>
+      <c r="E30" s="18">
+        <v>2.8840251239494101</v>
+      </c>
+      <c r="F30" s="18"/>
+      <c r="G30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="17">
+        <v>1.399</v>
+      </c>
+      <c r="I30" s="18">
+        <v>2.8979403803323001</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="K30" s="18">
+        <v>2.9638579807388399</v>
+      </c>
+      <c r="L30" s="17">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="M30" s="18">
+        <v>2.88007415821202</v>
+      </c>
+      <c r="N30" s="17">
+        <v>-0.36899999999999999</v>
+      </c>
+      <c r="O30" s="18">
+        <v>2.8776052675041401</v>
+      </c>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="17">
+        <v>1.6950000000000001</v>
+      </c>
+      <c r="R30" s="18">
+        <v>2.8859739092257599</v>
+      </c>
+      <c r="S30" s="17">
+        <v>1.403</v>
+      </c>
+      <c r="T30" s="18">
+        <v>2.88521236450838</v>
+      </c>
+      <c r="U30" s="17">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="V30" s="18">
+        <v>2.89360192713852</v>
+      </c>
+      <c r="W30" s="18"/>
+      <c r="X30" s="17">
+        <v>-0.94599999999999995</v>
+      </c>
+      <c r="Y30" s="18">
+        <v>2.8955572587538798</v>
+      </c>
+      <c r="Z30" s="17">
+        <v>2.9289999999999998</v>
+      </c>
+      <c r="AA30" s="18">
+        <v>2.9279464262705699</v>
+      </c>
+      <c r="AB30" s="17"/>
+      <c r="AC30" s="17">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="AD30" s="18">
+        <v>2.87913517233258</v>
+      </c>
+      <c r="AE30" s="17">
+        <v>0.155</v>
+      </c>
+      <c r="AF30" s="18">
+        <v>2.87832185176469</v>
+      </c>
+      <c r="AG30" s="17">
+        <v>0.501</v>
+      </c>
+      <c r="AH30" s="18">
+        <v>2.8817803047966102</v>
+      </c>
+      <c r="AI30" s="17"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="17">
+        <v>-7.6999999999999999E-2</v>
+      </c>
+      <c r="C31" s="18">
+        <v>0.34436126358876301</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E31" s="18">
+        <v>0.45186546121746601</v>
+      </c>
+      <c r="F31" s="18"/>
+      <c r="G31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="17">
+        <v>-0.35599999999999998</v>
+      </c>
+      <c r="I31" s="18">
+        <v>0.56838434992184195</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="K31" s="18">
+        <v>1.0992183888977201</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="M31" s="18">
+        <v>0.42598404042715698</v>
+      </c>
+      <c r="N31" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="O31" s="18">
+        <v>0.29885451080228898</v>
+      </c>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="17">
+        <v>0.436</v>
+      </c>
+      <c r="R31" s="18">
+        <v>0.41735974694905698</v>
+      </c>
+      <c r="S31" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="T31" s="18">
+        <v>0.46197139815357302</v>
+      </c>
+      <c r="U31" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="V31" s="18">
+        <v>0.469385575674233</v>
+      </c>
+      <c r="W31" s="18"/>
+      <c r="X31" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y31" s="18">
+        <v>0.653110283906572</v>
+      </c>
+      <c r="Z31" s="17">
+        <v>-0.79900000000000004</v>
+      </c>
+      <c r="AA31" s="18">
+        <v>0.70303119687451499</v>
+      </c>
+      <c r="AB31" s="17"/>
+      <c r="AC31" s="17">
+        <v>-0.13200000000000001</v>
+      </c>
+      <c r="AD31" s="18">
+        <v>0.31605038655219703</v>
+      </c>
+      <c r="AE31" s="17">
+        <v>-0.372</v>
+      </c>
+      <c r="AF31" s="18">
+        <v>0.30372352545264197</v>
+      </c>
+      <c r="AG31" s="17">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AH31" s="18">
+        <v>0.39702329086695498</v>
+      </c>
+      <c r="AI31" s="17"/>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="17">
+        <v>-0.113</v>
+      </c>
+      <c r="C32" s="18">
+        <v>0.34435842256184102</v>
+      </c>
+      <c r="D32" s="17">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="E32" s="18">
+        <v>0.45168191257814799</v>
+      </c>
+      <c r="F32" s="18"/>
+      <c r="G32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" s="17">
+        <v>-0.379</v>
+      </c>
+      <c r="I32" s="18">
+        <v>0.56886601155764904</v>
+      </c>
+      <c r="J32" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="K32" s="18">
+        <v>1.09927585724124</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="M32" s="18">
+        <v>0.42600942164025801</v>
+      </c>
+      <c r="N32" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="O32" s="18">
+        <v>0.29889288263081998</v>
+      </c>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="17">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="R32" s="18">
+        <v>0.41724732154495597</v>
+      </c>
+      <c r="S32" s="17">
+        <v>0.747</v>
+      </c>
+      <c r="T32" s="18">
+        <v>0.46173248424908903</v>
+      </c>
+      <c r="U32" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="V32" s="18">
+        <v>0.46925293543247898</v>
+      </c>
+      <c r="W32" s="18"/>
+      <c r="X32" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y32" s="18">
+        <v>0.65308418280025504</v>
+      </c>
+      <c r="Z32" s="17">
+        <v>-0.84199999999999997</v>
+      </c>
+      <c r="AA32" s="18">
+        <v>0.70292030858191301</v>
+      </c>
+      <c r="AB32" s="17"/>
+      <c r="AC32" s="17">
+        <v>-0.159</v>
+      </c>
+      <c r="AD32" s="18">
+        <v>0.31601806192486398</v>
+      </c>
+      <c r="AE32" s="17">
+        <v>-0.39500000000000002</v>
+      </c>
+      <c r="AF32" s="18">
+        <v>0.30370552432369002</v>
+      </c>
+      <c r="AG32" s="17">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="AH32" s="18">
+        <v>0.39700198384455798</v>
+      </c>
+      <c r="AI32" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="AC1:AH1"/>
+    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>